<commit_message>
saved estimates to an excel file to send to Yakima Nation.
</commit_message>
<xml_diff>
--- a/outgoing/estimates/PRO_est_Steelhead_2019_20200304.xlsx
+++ b/outgoing/estimates/PRO_est_Steelhead_2019_20200304.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seek/Documents/GitProjects/MyProjects/DabomYakimaSthd/outgoing/estimates/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C707DFE5-4776-4D45-91FB-67BD826CAA46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Escapement" sheetId="1" r:id="rId1"/>
     <sheet name="All Escapement" sheetId="2" r:id="rId2"/>
     <sheet name="Detection" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -231,8 +237,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +284,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -324,7 +338,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -356,9 +370,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -390,6 +422,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -565,7 +615,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -573,18 +623,17 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" customWidth="1"/>
-    <col min="5" max="5" width="2.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" customWidth="1"/>
+    <col min="5" max="5" width="2.83203125" customWidth="1"/>
+    <col min="6" max="7" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +656,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -630,21 +679,21 @@
         <v>332.3</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>159.8</v>
+        <v>159.80000000000001</v>
       </c>
       <c r="C3">
-        <v>157.7</v>
+        <v>157.69999999999999</v>
       </c>
       <c r="D3">
-        <v>156.3</v>
+        <v>156.30000000000001</v>
       </c>
       <c r="E3">
-        <v>37.3</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="F3">
         <v>84.4</v>
@@ -653,7 +702,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -676,7 +725,7 @@
         <v>437.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -684,13 +733,13 @@
         <v>163.5</v>
       </c>
       <c r="C5">
-        <v>159.7</v>
+        <v>159.69999999999999</v>
       </c>
       <c r="D5">
         <v>148.5</v>
       </c>
       <c r="E5">
-        <v>35.7</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="F5">
         <v>92.8</v>
@@ -699,7 +748,7 @@
         <v>233.6</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -710,7 +759,7 @@
         <v>87.3</v>
       </c>
       <c r="D6">
-        <v>72.6</v>
+        <v>72.599999999999994</v>
       </c>
       <c r="E6">
         <v>42.6</v>
@@ -728,7 +777,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -736,18 +785,17 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" customWidth="1"/>
-    <col min="5" max="5" width="2.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -770,7 +818,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -793,12 +841,12 @@
         <v>147.4</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3">
-        <v>20.4</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="C3">
         <v>17.3</v>
@@ -816,7 +864,7 @@
         <v>47.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -836,10 +884,10 @@
         <v>0.2</v>
       </c>
       <c r="G4">
-        <v>69.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>69.400000000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -862,7 +910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -885,7 +933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -905,10 +953,10 @@
         <v>0.7</v>
       </c>
       <c r="G7">
-        <v>38.8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>38.799999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -931,7 +979,7 @@
         <v>333.9</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -954,7 +1002,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -977,7 +1025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1000,7 +1048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1023,7 +1071,7 @@
         <v>255.1</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1037,7 +1085,7 @@
         <v>116.4</v>
       </c>
       <c r="E13">
-        <v>32.3</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="F13">
         <v>63.9</v>
@@ -1046,7 +1094,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1060,7 +1108,7 @@
         <v>768.1</v>
       </c>
       <c r="E14">
-        <v>152.2</v>
+        <v>152.19999999999999</v>
       </c>
       <c r="F14">
         <v>434.7</v>
@@ -1069,7 +1117,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1092,7 +1140,7 @@
         <v>332.3</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1103,7 +1151,7 @@
         <v>25</v>
       </c>
       <c r="D16">
-        <v>16.9</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="E16">
         <v>15.5</v>
@@ -1115,12 +1163,12 @@
         <v>56.3</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
       <c r="B17">
-        <v>542.7</v>
+        <v>542.70000000000005</v>
       </c>
       <c r="C17">
         <v>543.9</v>
@@ -1138,7 +1186,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1149,7 +1197,7 @@
         <v>87.3</v>
       </c>
       <c r="D18">
-        <v>72.6</v>
+        <v>72.599999999999994</v>
       </c>
       <c r="E18">
         <v>42.6</v>
@@ -1161,7 +1209,7 @@
         <v>168.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1184,7 +1232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1198,7 +1246,7 @@
         <v>18.8</v>
       </c>
       <c r="E20">
-        <v>18.1</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="F20">
         <v>3.4</v>
@@ -1207,21 +1255,21 @@
         <v>65.3</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
       <c r="B21">
-        <v>159.8</v>
+        <v>159.80000000000001</v>
       </c>
       <c r="C21">
-        <v>157.7</v>
+        <v>157.69999999999999</v>
       </c>
       <c r="D21">
-        <v>156.3</v>
+        <v>156.30000000000001</v>
       </c>
       <c r="E21">
-        <v>37.3</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="F21">
         <v>84.4</v>
@@ -1230,7 +1278,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1247,13 +1295,13 @@
         <v>80.3</v>
       </c>
       <c r="F22">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G22">
-        <v>274.1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>274.10000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -1276,7 +1324,7 @@
         <v>175.8</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1305,27 +1353,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" customWidth="1"/>
-    <col min="6" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" customWidth="1"/>
+    <col min="5" max="5" width="5.1640625" customWidth="1"/>
+    <col min="6" max="6" width="2.83203125" customWidth="1"/>
+    <col min="7" max="8" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -1351,7 +1398,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1359,25 +1406,25 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>0.889</v>
+        <v>0.88900000000000001</v>
       </c>
       <c r="D2">
-        <v>0.916</v>
+        <v>0.91600000000000004</v>
       </c>
       <c r="E2">
-        <v>0.962</v>
+        <v>0.96199999999999997</v>
       </c>
       <c r="F2">
-        <v>0.096</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="G2">
-        <v>0.696</v>
+        <v>0.69599999999999995</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1385,25 +1432,25 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>0.884</v>
+        <v>0.88400000000000001</v>
       </c>
       <c r="D3">
-        <v>0.915</v>
+        <v>0.91500000000000004</v>
       </c>
       <c r="E3">
-        <v>0.961</v>
+        <v>0.96099999999999997</v>
       </c>
       <c r="F3">
-        <v>0.103</v>
+        <v>0.10299999999999999</v>
       </c>
       <c r="G3">
-        <v>0.664</v>
+        <v>0.66400000000000003</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1429,7 +1476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1437,25 +1484,25 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0.589</v>
+        <v>0.58899999999999997</v>
       </c>
       <c r="D5">
-        <v>0.608</v>
+        <v>0.60799999999999998</v>
       </c>
       <c r="E5">
         <v>0.879</v>
       </c>
       <c r="F5">
-        <v>0.262</v>
+        <v>0.26200000000000001</v>
       </c>
       <c r="G5">
-        <v>0.141</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="H5">
         <v>0.998</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1463,25 +1510,25 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0.595</v>
+        <v>0.59499999999999997</v>
       </c>
       <c r="D6">
-        <v>0.613</v>
+        <v>0.61299999999999999</v>
       </c>
       <c r="E6">
-        <v>0.719</v>
+        <v>0.71899999999999997</v>
       </c>
       <c r="F6">
         <v>0.253</v>
       </c>
       <c r="G6">
-        <v>0.145</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="H6">
         <v>0.998</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1507,7 +1554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1533,7 +1580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -1541,25 +1588,25 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0.772</v>
+        <v>0.77200000000000002</v>
       </c>
       <c r="D9">
-        <v>0.819</v>
+        <v>0.81899999999999995</v>
       </c>
       <c r="E9">
-        <v>0.891</v>
+        <v>0.89100000000000001</v>
       </c>
       <c r="F9">
         <v>0.18</v>
       </c>
       <c r="G9">
-        <v>0.414</v>
+        <v>0.41399999999999998</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -1567,25 +1614,25 @@
         <v>3</v>
       </c>
       <c r="C10">
-        <v>0.778</v>
+        <v>0.77800000000000002</v>
       </c>
       <c r="D10">
-        <v>0.822</v>
+        <v>0.82199999999999995</v>
       </c>
       <c r="E10">
-        <v>0.906</v>
+        <v>0.90600000000000003</v>
       </c>
       <c r="F10">
-        <v>0.173</v>
+        <v>0.17299999999999999</v>
       </c>
       <c r="G10">
-        <v>0.422</v>
+        <v>0.42199999999999999</v>
       </c>
       <c r="H10">
         <v>0.999</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -1593,25 +1640,25 @@
         <v>12</v>
       </c>
       <c r="C11">
-        <v>0.927</v>
+        <v>0.92700000000000005</v>
       </c>
       <c r="D11">
-        <v>0.945</v>
+        <v>0.94499999999999995</v>
       </c>
       <c r="E11">
-        <v>0.979</v>
+        <v>0.97899999999999998</v>
       </c>
       <c r="F11">
-        <v>0.067</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="G11">
-        <v>0.793</v>
+        <v>0.79300000000000004</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1619,25 +1666,25 @@
         <v>12</v>
       </c>
       <c r="C12">
-        <v>0.929</v>
+        <v>0.92900000000000005</v>
       </c>
       <c r="D12">
         <v>0.95</v>
       </c>
       <c r="E12">
-        <v>0.983</v>
+        <v>0.98299999999999998</v>
       </c>
       <c r="F12">
-        <v>0.069</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="G12">
-        <v>0.792</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -1645,13 +1692,13 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>0.581</v>
+        <v>0.58099999999999996</v>
       </c>
       <c r="D13">
-        <v>0.586</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="E13">
-        <v>0.597</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="F13">
         <v>0.123</v>
@@ -1660,10 +1707,10 @@
         <v>0.35</v>
       </c>
       <c r="H13">
-        <v>0.798</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>0.79800000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -1671,25 +1718,25 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>0.635</v>
+        <v>0.63500000000000001</v>
       </c>
       <c r="D14">
-        <v>0.639</v>
+        <v>0.63900000000000001</v>
       </c>
       <c r="E14">
-        <v>0.653</v>
+        <v>0.65300000000000002</v>
       </c>
       <c r="F14">
-        <v>0.119</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="G14">
-        <v>0.424</v>
+        <v>0.42399999999999999</v>
       </c>
       <c r="H14">
-        <v>0.884</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>0.88400000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -1697,25 +1744,25 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <v>0.723</v>
+        <v>0.72299999999999998</v>
       </c>
       <c r="D15">
-        <v>0.764</v>
+        <v>0.76400000000000001</v>
       </c>
       <c r="E15">
-        <v>0.909</v>
+        <v>0.90900000000000003</v>
       </c>
       <c r="F15">
         <v>0.2</v>
       </c>
       <c r="G15">
-        <v>0.332</v>
+        <v>0.33200000000000002</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -1723,25 +1770,25 @@
         <v>2</v>
       </c>
       <c r="C16">
-        <v>0.725</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="D16">
-        <v>0.763</v>
+        <v>0.76300000000000001</v>
       </c>
       <c r="E16">
-        <v>0.909</v>
+        <v>0.90900000000000003</v>
       </c>
       <c r="F16">
-        <v>0.201</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="G16">
-        <v>0.337</v>
+        <v>0.33700000000000002</v>
       </c>
       <c r="H16">
         <v>0.999</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -1755,19 +1802,19 @@
         <v>0.253</v>
       </c>
       <c r="E17">
-        <v>0.238</v>
+        <v>0.23799999999999999</v>
       </c>
       <c r="F17">
-        <v>0.059</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="G17">
-        <v>0.147</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="H17">
         <v>0.378</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -1775,25 +1822,25 @@
         <v>14</v>
       </c>
       <c r="C18">
-        <v>0.274</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="D18">
-        <v>0.272</v>
+        <v>0.27200000000000002</v>
       </c>
       <c r="E18">
-        <v>0.272</v>
+        <v>0.27200000000000002</v>
       </c>
       <c r="F18">
-        <v>0.059</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="G18">
-        <v>0.168</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="H18">
-        <v>0.402</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>0.40200000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1801,25 +1848,25 @@
         <v>2</v>
       </c>
       <c r="C19">
-        <v>0.697</v>
+        <v>0.69699999999999995</v>
       </c>
       <c r="D19">
-        <v>0.731</v>
+        <v>0.73099999999999998</v>
       </c>
       <c r="E19">
-        <v>0.908</v>
+        <v>0.90800000000000003</v>
       </c>
       <c r="F19">
         <v>0.215</v>
       </c>
       <c r="G19">
-        <v>0.286</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="H19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -1827,25 +1874,25 @@
         <v>2</v>
       </c>
       <c r="C20">
-        <v>0.697</v>
+        <v>0.69699999999999995</v>
       </c>
       <c r="D20">
         <v>0.74</v>
       </c>
       <c r="E20">
-        <v>0.896</v>
+        <v>0.89600000000000002</v>
       </c>
       <c r="F20">
         <v>0.216</v>
       </c>
       <c r="G20">
-        <v>0.293</v>
+        <v>0.29299999999999998</v>
       </c>
       <c r="H20">
         <v>0.999</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -1853,25 +1900,25 @@
         <v>11</v>
       </c>
       <c r="C21">
-        <v>0.704</v>
+        <v>0.70399999999999996</v>
       </c>
       <c r="D21">
-        <v>0.712</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="E21">
-        <v>0.714</v>
+        <v>0.71399999999999997</v>
       </c>
       <c r="F21">
         <v>0.107</v>
       </c>
       <c r="G21">
-        <v>0.484</v>
+        <v>0.48399999999999999</v>
       </c>
       <c r="H21">
-        <v>0.888</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>0.88800000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>56</v>
       </c>
@@ -1882,22 +1929,22 @@
         <v>0.879</v>
       </c>
       <c r="D22">
-        <v>0.896</v>
+        <v>0.89600000000000002</v>
       </c>
       <c r="E22">
-        <v>0.933</v>
+        <v>0.93300000000000005</v>
       </c>
       <c r="F22">
-        <v>0.078</v>
+        <v>7.8E-2</v>
       </c>
       <c r="G22">
-        <v>0.727</v>
+        <v>0.72699999999999998</v>
       </c>
       <c r="H22">
         <v>0.99</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>57</v>
       </c>
@@ -1905,25 +1952,25 @@
         <v>12</v>
       </c>
       <c r="C23">
-        <v>0.924</v>
+        <v>0.92400000000000004</v>
       </c>
       <c r="D23">
-        <v>0.942</v>
+        <v>0.94199999999999995</v>
       </c>
       <c r="E23">
-        <v>0.979</v>
+        <v>0.97899999999999998</v>
       </c>
       <c r="F23">
-        <v>0.07</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G23">
-        <v>0.789</v>
+        <v>0.78900000000000003</v>
       </c>
       <c r="H23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>58</v>
       </c>
@@ -1931,25 +1978,25 @@
         <v>11</v>
       </c>
       <c r="C24">
-        <v>0.848</v>
+        <v>0.84799999999999998</v>
       </c>
       <c r="D24">
-        <v>0.863</v>
+        <v>0.86299999999999999</v>
       </c>
       <c r="E24">
-        <v>0.892</v>
+        <v>0.89200000000000002</v>
       </c>
       <c r="F24">
-        <v>0.091</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="G24">
-        <v>0.664</v>
+        <v>0.66400000000000003</v>
       </c>
       <c r="H24">
-        <v>0.985</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>0.98499999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -1975,7 +2022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>60</v>
       </c>
@@ -2001,7 +2048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -2027,7 +2074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>62</v>
       </c>
@@ -2053,7 +2100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -2079,7 +2126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -2105,7 +2152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -2131,7 +2178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -2157,7 +2204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -2183,7 +2230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>67</v>
       </c>
@@ -2209,7 +2256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>68</v>
       </c>
@@ -2235,7 +2282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>69</v>
       </c>

</xml_diff>